<commit_message>
Merged PR 7758: PRI23251: sending daypart code to DS
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Program lineup/ProgramLineupExport.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Program lineup/ProgramLineupExport.xlsx
@@ -81,7 +81,7 @@
   </si>
   <si>
     <t xml:space="preserve">Report generated on 4/4/20
-Estimate as of 3/6/20</t>
+Estimate as of 3/7/20</t>
   </si>
   <si>
     <t>Stub Agency</t>
@@ -144,7 +144,7 @@
     <t>CHILDREN</t>
   </si>
   <si>
-    <t>LF</t>
+    <t>MDN</t>
   </si>
   <si>
     <t>Even</t>
@@ -1343,7 +1343,7 @@
       <c r="J2" s="46" t="str">
         <f>'Detailed View'!J2</f>
         <v>Report generated on 4/4/20
-Estimate as of 3/6/20</v>
+Estimate as of 3/7/20</v>
       </c>
       <c r="K2" s="46"/>
       <c r="L2" s="21"/>
@@ -1869,7 +1869,7 @@
       <c r="J2" s="46" t="str">
         <f>'Detailed View'!J2</f>
         <v>Report generated on 4/4/20
-Estimate as of 3/6/20</v>
+Estimate as of 3/7/20</v>
       </c>
       <c r="K2" s="46"/>
       <c r="L2" s="21"/>

</xml_diff>

<commit_message>
Merged PR 9457: BP-1102 Update program line Markets allocation display
BP-1102 Implementation and testing
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Program lineup/ProgramLineupExport.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Program lineup/ProgramLineupExport.xlsx
@@ -1,24 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sroibu\Source\Repos\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AC51127F-2340-4034-9F92-958451ACD423}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA89CAF-C7EF-4B81-A7B3-67F2103E0D62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="23250" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
+    <workbookView xWindow="28680" yWindow="435" windowWidth="25440" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Default View" sheetId="7" r:id="rId1"/>
     <sheet name="Allocations" sheetId="6" r:id="rId2"/>
     <sheet name="Detailed View" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017" fullCalcOnLoad="1" calcMode="auto"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1" calcMode="auto"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mgMtMfamHb1jVya39tpwhGUN2dNvA=="/>
     </ext>
@@ -27,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>*This Program Lineup is subject to change.</t>
   </si>
@@ -56,32 +64,65 @@
     <t>Client Contact</t>
   </si>
   <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Genre</t>
+  </si>
+  <si>
+    <t>No. of Stations</t>
+  </si>
+  <si>
+    <t>No. of DMAs</t>
+  </si>
+  <si>
+    <t>EARLY NEWS</t>
+  </si>
+  <si>
+    <t>CHILDREN</t>
+  </si>
+  <si>
+    <t>Even</t>
+  </si>
+  <si>
+    <t>LATE NEWS</t>
+  </si>
+  <si>
+    <t>COMEDY</t>
+  </si>
+  <si>
     <t>Allocation by Daypart</t>
   </si>
   <si>
     <t>Daypart</t>
   </si>
   <si>
-    <t>Weight</t>
+    <t>MDN</t>
   </si>
   <si>
     <t>Allocation by Genre</t>
   </si>
   <si>
-    <t>Genre</t>
-  </si>
-  <si>
     <t>Allocation by DMA</t>
   </si>
   <si>
     <t>DMA</t>
   </si>
   <si>
+    <t>NEW YORK</t>
+  </si>
+  <si>
+    <t>PORTLAND-AUBURN</t>
+  </si>
+  <si>
     <t>Plan Pricing 2 | Program Lineup*</t>
   </si>
   <si>
     <t xml:space="preserve">Report generated on 4/4/20
-Estimate as of 3/7/20</t>
+Estimate as of 8/5/20</t>
   </si>
   <si>
     <t>Stub Agency</t>
@@ -120,12 +161,6 @@
     <t>Time Periods</t>
   </si>
   <si>
-    <t>Program</t>
-  </si>
-  <si>
-    <t>NEW YORK</t>
-  </si>
-  <si>
     <t>WPIX</t>
   </si>
   <si>
@@ -138,49 +173,19 @@
     <t>12AM-12:30AM</t>
   </si>
   <si>
-    <t>EARLY NEWS</t>
-  </si>
-  <si>
-    <t>CHILDREN</t>
-  </si>
-  <si>
-    <t>MDN</t>
-  </si>
-  <si>
-    <t>Even</t>
-  </si>
-  <si>
-    <t>12:30AM-1AM</t>
-  </si>
-  <si>
     <t>SA</t>
   </si>
   <si>
     <t>SU</t>
   </si>
   <si>
-    <t>12AM-1AM</t>
-  </si>
-  <si>
-    <t>PORTLAND-AUBURN</t>
+    <t>12AM-12:33AM</t>
   </si>
   <si>
     <t>WPFO</t>
   </si>
   <si>
     <t>FOX</t>
-  </si>
-  <si>
-    <t>LATE NEWS</t>
-  </si>
-  <si>
-    <t>COMEDY</t>
-  </si>
-  <si>
-    <t>No. of Stations</t>
-  </si>
-  <si>
-    <t>No. of DMAs</t>
   </si>
 </sst>
 </file>
@@ -502,170 +507,191 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="2" applyBorder="1" xfId="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+  <cellXfs count="68">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="2" applyBorder="1" xfId="1" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="2" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="3" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="4" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="7" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="3" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="4" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="9" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="9" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="3" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="9" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="9" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="3" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="3" applyFill="1" borderId="2" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="3" applyFill="1" borderId="6" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="10" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="11" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="11" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="3" applyFill="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="3" applyFill="1" borderId="6" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="10" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="11" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="11" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="10" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="10" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="6" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="5" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="9" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="11" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="6" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="5" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="9" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="11" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="10" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="12" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="9" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="10" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="12" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="9" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="8" applyFont="1" fillId="2" applyFill="1" borderId="7" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="8" applyFont="1" fillId="2" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="8" applyFont="1" fillId="2" applyFill="1" borderId="8" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="8" applyFont="1" fillId="2" applyFill="1" borderId="8" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="3" applyBorder="1" xfId="0"/>
-    <xf numFmtId="9" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="6" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="3" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="9" applyNumberFormat="1" fontId="7" applyFont="1" fillId="0" applyFill="1" borderId="6" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="0" applyFill="1" borderId="3" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="3" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="0" applyFill="1" borderId="3" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="5" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="10" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="11" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="11" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="14" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="13" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="13" applyFont="1" fillId="0" applyFill="1" borderId="5" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="10" applyNumberFormat="1" fontId="7" applyFont="1" fillId="0" applyFill="1" borderId="6" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="9" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="10" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="10" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="11" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="12" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="13" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="14" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="15" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="14" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="15" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="16" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="17" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="9" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="6" applyBorder="1" xfId="0">
+    <xf numFmtId="9" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="10" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="11" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="5" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="10" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="11" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="11" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="14" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0">
-      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="13" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="13" applyFont="1" fillId="0" applyFill="1" borderId="5" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="9" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="10" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="10" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="11" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="12" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="13" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="14" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="15" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="14" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="15" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="16" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="17" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="13" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="15" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="17" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="9" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="0" applyFill="1" borderId="10" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="10" applyNumberFormat="1" fontId="7" applyFont="1" fillId="0" applyFill="1" borderId="11" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="13" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="0" applyFill="1" borderId="15" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="10" applyNumberFormat="1" fontId="7" applyFont="1" fillId="0" applyFill="1" borderId="17" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="10" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="11" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="10" applyNumberFormat="1" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="17" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
@@ -673,112 +699,7 @@
     <cellStyle name="Header" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -834,13 +755,13 @@
   </dxfs>
   <tableStyles count="3" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="20"/>
+      <tableStyleElement type="wholeTable" dxfId="5"/>
     </tableStyle>
     <tableStyle name="Table Style 2" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="firstRowStripe" dxfId="19"/>
+      <tableStyleElement type="firstRowStripe" dxfId="4"/>
     </tableStyle>
     <tableStyle name="Table Style 3" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
-      <tableStyleElement type="firstRowStripe" dxfId="18"/>
+      <tableStyleElement type="firstRowStripe" dxfId="3"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1306,7 +1227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M111"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="0" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C6" sqref="C6:D6"/>
     </sheetView>
@@ -1340,25 +1261,25 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-      <c r="J2" s="46" t="str">
+      <c r="J2" s="38" t="str">
         <f>'Detailed View'!J2</f>
         <v>Report generated on 4/4/20
-Estimate as of 3/7/20</v>
-      </c>
-      <c r="K2" s="46"/>
+Estimate as of 8/5/20</v>
+      </c>
+      <c r="K2" s="38"/>
       <c r="L2" s="21"/>
       <c r="M2" s="2"/>
     </row>
     <row r="3" ht="16.15" customHeight="1">
       <c r="B3" s="2"/>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -1378,10 +1299,10 @@
       <c r="M4" s="2"/>
     </row>
     <row r="5" ht="18" customHeight="1" s="15" customFormat="1">
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="43"/>
+      <c r="D5" s="35"/>
       <c r="E5" s="27" t="s">
         <v>2</v>
       </c>
@@ -1406,20 +1327,20 @@
       </c>
     </row>
     <row r="6" ht="18" customHeight="1" s="16" customFormat="1">
-      <c r="C6" s="44" t="e">
+      <c r="C6" s="36" t="e">
         <f>'Detailed View'!C6:D6</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D6" s="44"/>
+      <c r="D6" s="36"/>
       <c r="E6" s="26" t="str">
         <f>'Detailed View'!E6</f>
         <v>Stub Advertiser</v>
       </c>
-      <c r="F6" s="45" t="e">
+      <c r="F6" s="37" t="e">
         <f>'Detailed View'!F6:G6</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G6" s="45"/>
+      <c r="G6" s="37"/>
       <c r="H6" s="26" t="str">
         <f>'Detailed View'!H6</f>
         <v>HH</v>
@@ -1443,32 +1364,63 @@
     <row r="8" ht="24" customHeight="1">
       <c r="C8" s="5"/>
       <c r="D8" s="4" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="I8" s="6"/>
     </row>
     <row r="9" ht="24" customHeight="1" s="25" customFormat="1">
-      <c r="C9" s="39"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="41"/>
-    </row>
-    <row r="10" ht="24" customHeight="1" s="25" customFormat="1"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="55">
+        <v>0.99100112485939262</v>
+      </c>
+      <c r="F9" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="43">
+        <v>1</v>
+      </c>
+      <c r="H9" s="43">
+        <v>1</v>
+      </c>
+      <c r="I9" s="56"/>
+    </row>
+    <row r="10" ht="24" customHeight="1" s="25" customFormat="1">
+      <c r="A10" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="57"/>
+      <c r="D10" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="58">
+        <v>0.0089988751406074249</v>
+      </c>
+      <c r="F10" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="49">
+        <v>1</v>
+      </c>
+      <c r="H10" s="49">
+        <v>1</v>
+      </c>
+      <c r="I10" s="59"/>
+    </row>
     <row r="11" ht="24" customHeight="1" s="25" customFormat="1"/>
     <row r="12" ht="24" customHeight="1" s="25" customFormat="1"/>
     <row r="13" ht="24" customHeight="1" s="25" customFormat="1"/>
@@ -1806,7 +1758,7 @@
       <c r="K111" s="8"/>
     </row>
   </sheetData>
-  <sortState ref="D9:I26">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D9:I26">
     <sortCondition descending="1" ref="E9:E26"/>
   </sortState>
   <mergeCells>
@@ -1830,7 +1782,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:M105"/>
+  <dimension ref="A2:M107"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0" tabSelected="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
@@ -1866,25 +1818,25 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-      <c r="J2" s="46" t="str">
+      <c r="J2" s="38" t="str">
         <f>'Detailed View'!J2</f>
         <v>Report generated on 4/4/20
-Estimate as of 3/7/20</v>
-      </c>
-      <c r="K2" s="46"/>
+Estimate as of 8/5/20</v>
+      </c>
+      <c r="K2" s="38"/>
       <c r="L2" s="21"/>
       <c r="M2" s="2"/>
     </row>
     <row r="3" ht="16.15" customHeight="1">
       <c r="B3" s="2"/>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -1904,10 +1856,10 @@
       <c r="M4" s="2"/>
     </row>
     <row r="5" ht="18" customHeight="1" s="15" customFormat="1">
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="43"/>
+      <c r="D5" s="35"/>
       <c r="E5" s="27" t="s">
         <v>2</v>
       </c>
@@ -1932,20 +1884,20 @@
       </c>
     </row>
     <row r="6" ht="18" customHeight="1" s="16" customFormat="1">
-      <c r="C6" s="44" t="str">
+      <c r="C6" s="36" t="str">
         <f>'Detailed View'!C6</f>
         <v>Stub Agency</v>
       </c>
-      <c r="D6" s="44"/>
+      <c r="D6" s="36"/>
       <c r="E6" s="26" t="str">
         <f>'Detailed View'!E6</f>
         <v>Stub Advertiser</v>
       </c>
-      <c r="F6" s="45" t="str">
+      <c r="F6" s="37" t="str">
         <f>'Detailed View'!F6</f>
         <v>10/01/18 - 10/31/18</v>
       </c>
-      <c r="G6" s="45"/>
+      <c r="G6" s="37"/>
       <c r="H6" s="26" t="str">
         <f>'Detailed View'!H6</f>
         <v>HH</v>
@@ -1969,27 +1921,31 @@
     <row r="8" ht="24" customHeight="1"/>
     <row r="9" ht="24" customHeight="1">
       <c r="A9" s="23"/>
-      <c r="C9" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
+      <c r="C9" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
     </row>
     <row r="10" ht="24" customHeight="1">
       <c r="A10" s="23"/>
       <c r="C10" s="5"/>
       <c r="D10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="22" t="s">
         <v>10</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="11" ht="24" customHeight="1">
       <c r="A11" s="23"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="37"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="41">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" ht="24" customHeight="1">
       <c r="A12" s="23"/>
@@ -1999,68 +1955,94 @@
     </row>
     <row r="13" ht="24" customHeight="1">
       <c r="A13" s="23"/>
-      <c r="C13" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
+      <c r="C13" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
     </row>
     <row r="14" ht="24" customHeight="1">
       <c r="A14" s="23"/>
       <c r="C14" s="5"/>
       <c r="D14" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" ht="24" customHeight="1">
       <c r="A15" s="23"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="34"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="66">
+        <v>0.99100112485939262</v>
+      </c>
     </row>
     <row r="16" ht="24" customHeight="1">
-      <c r="A16" s="23"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
+      <c r="A16" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="63"/>
+      <c r="D16" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="67">
+        <v>0.0089988751406074249</v>
+      </c>
     </row>
     <row r="17" ht="24" customHeight="1">
       <c r="A17" s="23"/>
-      <c r="C17" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
     </row>
     <row r="18" ht="24" customHeight="1">
       <c r="A18" s="23"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>11</v>
-      </c>
+      <c r="C18" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
     </row>
     <row r="19" ht="24" customHeight="1">
       <c r="A19" s="23"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="37"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" ht="24" customHeight="1">
       <c r="A20" s="23"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="61" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="62">
+        <v>0.99100112485939262</v>
+      </c>
     </row>
     <row r="21" ht="24" customHeight="1">
-      <c r="A21" s="23"/>
-    </row>
-    <row r="22" ht="15" customHeight="1">
+      <c r="A21" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="63"/>
+      <c r="D21" s="64" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="65">
+        <v>0.0089988751406074249</v>
+      </c>
+    </row>
+    <row r="22" ht="24" customHeight="1">
       <c r="A22" s="23"/>
     </row>
-    <row r="23" ht="15" customHeight="1">
+    <row r="23" ht="24" customHeight="1">
       <c r="A23" s="23"/>
     </row>
     <row r="24" ht="15" customHeight="1">
@@ -2240,13 +2222,11 @@
     <row r="82" ht="15" customHeight="1">
       <c r="A82" s="23"/>
     </row>
-    <row r="83" ht="15" customHeight="1" s="25" customFormat="1">
-      <c r="K83" s="10"/>
-      <c r="L83" s="10"/>
-    </row>
-    <row r="84" ht="15" customHeight="1" s="25" customFormat="1">
-      <c r="K84" s="10"/>
-      <c r="L84" s="10"/>
+    <row r="83" ht="15" customHeight="1">
+      <c r="A83" s="23"/>
+    </row>
+    <row r="84" ht="15" customHeight="1">
+      <c r="A84" s="23"/>
     </row>
     <row r="85" ht="15" customHeight="1" s="25" customFormat="1">
       <c r="K85" s="10"/>
@@ -2300,11 +2280,13 @@
       <c r="K97" s="10"/>
       <c r="L97" s="10"/>
     </row>
-    <row r="98" ht="15" customHeight="1">
-      <c r="K98" s="8"/>
-    </row>
-    <row r="99" ht="15" customHeight="1">
-      <c r="K99" s="8"/>
+    <row r="98" ht="15" customHeight="1" s="25" customFormat="1">
+      <c r="K98" s="10"/>
+      <c r="L98" s="10"/>
+    </row>
+    <row r="99" ht="15" customHeight="1" s="25" customFormat="1">
+      <c r="K99" s="10"/>
+      <c r="L99" s="10"/>
     </row>
     <row r="100" ht="15" customHeight="1">
       <c r="K100" s="8"/>
@@ -2323,13 +2305,19 @@
     </row>
     <row r="105" ht="15" customHeight="1">
       <c r="K105" s="8"/>
+    </row>
+    <row r="106" ht="15" customHeight="1">
+      <c r="K106" s="8"/>
+    </row>
+    <row r="107" ht="15" customHeight="1">
+      <c r="K107" s="8"/>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
     <mergeCell ref="E3:J3"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
@@ -2382,29 +2370,29 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="28" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-      <c r="J2" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="46"/>
+      <c r="J2" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="38"/>
       <c r="L2" s="21"/>
       <c r="M2" s="2"/>
       <c r="O2" s="23"/>
     </row>
     <row r="3" ht="16.15" customHeight="1">
       <c r="B3" s="2"/>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -2412,12 +2400,12 @@
     </row>
     <row r="4" ht="16.15" customHeight="1">
       <c r="B4" s="2"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
       <c r="K4" s="19"/>
@@ -2425,10 +2413,10 @@
       <c r="M4" s="2"/>
     </row>
     <row r="5" ht="18" customHeight="1" s="15" customFormat="1">
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="43"/>
+      <c r="D5" s="35"/>
       <c r="E5" s="20" t="s">
         <v>2</v>
       </c>
@@ -2453,350 +2441,270 @@
       </c>
     </row>
     <row r="6" ht="18" customHeight="1" s="16" customFormat="1">
-      <c r="C6" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="44"/>
+      <c r="C6" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="36"/>
       <c r="E6" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="45" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="45"/>
+        <v>30</v>
+      </c>
+      <c r="F6" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="37"/>
       <c r="H6" s="17" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="M6" s="17"/>
     </row>
     <row r="8" ht="24" customHeight="1">
       <c r="B8" s="7"/>
       <c r="C8" s="11" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L8" s="3"/>
     </row>
     <row r="9" ht="24" customHeight="1" s="25" customFormat="1">
       <c r="B9" s="30"/>
-      <c r="C9" s="49">
+      <c r="C9" s="42">
         <v>1</v>
       </c>
-      <c r="D9" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="50" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" s="50" t="s">
-        <v>36</v>
-      </c>
-      <c r="J9" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="K9" s="52" t="s">
-        <v>38</v>
+      <c r="D9" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="45" t="s">
+        <v>21</v>
       </c>
       <c r="L9" s="31"/>
     </row>
     <row r="10" ht="24" customHeight="1" s="9" customFormat="1">
       <c r="A10" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="53">
+        <v>16</v>
+      </c>
+      <c r="C10" s="46">
         <v>1</v>
       </c>
-      <c r="D10" s="55" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="55" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="55" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="55" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="57" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" s="55" t="s">
-        <v>36</v>
-      </c>
-      <c r="J10" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="K10" s="59" t="s">
-        <v>38</v>
+      <c r="D10" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" s="52" t="s">
+        <v>21</v>
       </c>
       <c r="L10" s="10"/>
     </row>
     <row r="11" ht="24" customHeight="1" s="9" customFormat="1">
       <c r="A11" s="25"/>
-      <c r="C11" s="53">
+      <c r="C11" s="46">
         <v>1</v>
       </c>
-      <c r="D11" s="55" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="55" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="55" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="55" t="s">
+      <c r="D11" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="I11" s="55" t="s">
-        <v>36</v>
-      </c>
-      <c r="J11" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="K11" s="59" t="s">
-        <v>38</v>
+      <c r="F11" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="50" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" s="52" t="s">
+        <v>21</v>
       </c>
       <c r="L11" s="10"/>
     </row>
     <row r="12" ht="24" customHeight="1" s="9" customFormat="1">
       <c r="A12" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="53">
-        <v>1</v>
-      </c>
-      <c r="D12" s="55" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="55" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="55" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="55" t="s">
-        <v>41</v>
-      </c>
-      <c r="H12" s="57" t="s">
-        <v>40</v>
-      </c>
-      <c r="I12" s="55" t="s">
-        <v>36</v>
-      </c>
-      <c r="J12" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="K12" s="59" t="s">
-        <v>38</v>
+        <v>16</v>
+      </c>
+      <c r="C12" s="46">
+        <v>79</v>
+      </c>
+      <c r="D12" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="52" t="s">
+        <v>21</v>
       </c>
       <c r="L12" s="10"/>
     </row>
     <row r="13" ht="24" customHeight="1" s="9" customFormat="1">
       <c r="A13" s="25"/>
-      <c r="C13" s="53">
-        <v>1</v>
-      </c>
-      <c r="D13" s="55" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="55" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="55" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="55" t="s">
-        <v>42</v>
-      </c>
-      <c r="H13" s="57" t="s">
-        <v>43</v>
-      </c>
-      <c r="I13" s="55" t="s">
-        <v>36</v>
-      </c>
-      <c r="J13" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="K13" s="59" t="s">
-        <v>38</v>
+      <c r="C13" s="46">
+        <v>79</v>
+      </c>
+      <c r="D13" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="50" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="K13" s="52" t="s">
+        <v>21</v>
       </c>
       <c r="L13" s="10"/>
     </row>
     <row r="14" ht="24" customHeight="1" s="9" customFormat="1">
       <c r="A14" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="53">
+        <v>16</v>
+      </c>
+      <c r="C14" s="47">
         <v>79</v>
       </c>
-      <c r="D14" s="55" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" s="55" t="s">
+      <c r="D14" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="55" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" s="55" t="s">
+      <c r="H14" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="J14" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="K14" s="59" t="s">
-        <v>38</v>
+      <c r="I14" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="53" t="s">
+        <v>21</v>
       </c>
       <c r="L14" s="10"/>
     </row>
-    <row r="15" ht="24" customHeight="1" s="9" customFormat="1">
+    <row r="15" ht="15" customHeight="1" s="9" customFormat="1">
       <c r="A15" s="25"/>
-      <c r="C15" s="53">
-        <v>79</v>
-      </c>
-      <c r="D15" s="55" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="55" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" s="55" t="s">
-        <v>41</v>
-      </c>
-      <c r="H15" s="57" t="s">
-        <v>43</v>
-      </c>
-      <c r="I15" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="J15" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="K15" s="59" t="s">
-        <v>38</v>
-      </c>
+      <c r="K15" s="10"/>
       <c r="L15" s="10"/>
     </row>
-    <row r="16" ht="24" customHeight="1" s="9" customFormat="1">
-      <c r="A16" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="53">
-        <v>79</v>
-      </c>
-      <c r="D16" s="55" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="55" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="55" t="s">
-        <v>42</v>
-      </c>
-      <c r="H16" s="57" t="s">
-        <v>43</v>
-      </c>
-      <c r="I16" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="J16" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="K16" s="59" t="s">
-        <v>38</v>
-      </c>
+    <row r="16" ht="15" customHeight="1" s="9" customFormat="1">
+      <c r="A16" s="25"/>
+      <c r="K16" s="10"/>
       <c r="L16" s="10"/>
     </row>
-    <row r="17" ht="24" customHeight="1" s="9" customFormat="1">
+    <row r="17" ht="15" customHeight="1" s="9" customFormat="1">
       <c r="A17" s="25"/>
-      <c r="C17" s="54">
-        <v>79</v>
-      </c>
-      <c r="D17" s="56" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="56" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" s="56" t="s">
-        <v>46</v>
-      </c>
-      <c r="G17" s="56" t="s">
-        <v>34</v>
-      </c>
-      <c r="H17" s="58" t="s">
-        <v>40</v>
-      </c>
-      <c r="I17" s="56" t="s">
-        <v>47</v>
-      </c>
-      <c r="J17" s="56" t="s">
-        <v>48</v>
-      </c>
-      <c r="K17" s="60" t="s">
-        <v>38</v>
-      </c>
+      <c r="K17" s="10"/>
       <c r="L17" s="10"/>
     </row>
     <row r="18" ht="15" customHeight="1" s="9" customFormat="1">
@@ -3185,6 +3093,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000192CE90DA120240A67EE82BE1FBFF43" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="623d129459d6fae29ac2c5d491c3782f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e2beb7e-37df-4602-aab8-4f6673c75e9a" xmlns:ns4="eaec1813-26bf-4c98-9021-907af21e1945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfd2e6b22ac1ad737273b5b960116aad" ns3:_="" ns4:_="">
     <xsd:import namespace="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
@@ -3407,12 +3321,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3423,6 +3331,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{022D3F0F-7ADC-46CC-B0CC-F40745AEE35B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{060BAEE3-07B5-4CCF-A906-7A824BD2B0D7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3441,15 +3358,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{022D3F0F-7ADC-46CC-B0CC-F40745AEE35B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02D4F406-DB10-4FCE-90E8-E4689C9E60D8}">
   <ds:schemaRefs>

</xml_diff>